<commit_message>
feat: cambio de contraseña por usuario desde navbar
</commit_message>
<xml_diff>
--- a/database/usuarios.xlsx
+++ b/database/usuarios.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>consulta1</t>
+  </si>
+  <si>
+    <t>tero2050</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,8 +439,8 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>1234</v>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>